<commit_message>
Changes to be committed: 	modified:   TestCase.xlsx
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
   <si>
     <t>ICカードで改札を通過するユースケースのテスト</t>
   </si>
@@ -23,10 +23,16 @@
     <t>チャージ額</t>
   </si>
   <si>
-    <t>駅</t>
+    <t>ICカードの駅</t>
+  </si>
+  <si>
+    <t>改札駅</t>
   </si>
   <si>
     <t>Gate</t>
+  </si>
+  <si>
+    <t>Shinjuku</t>
   </si>
   <si>
     <t>Takadanobaba</t>
@@ -41,11 +47,17 @@
     <t>開く</t>
   </si>
   <si>
-    <t>iidabashi</t>
+    <t>null</t>
   </si>
   <si>
     <t>閉じる（ エラー）</t>
+  </si>
+  <si>
+    <t>閉じる（料金不足）</t>
+  </si>
+  <si>
+    <t>iidabashi</t>
   </si>
 </sst>
 </file>
@@ -55,7 +67,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -67,42 +79,92 @@
       <name val="ヒラギノ角ゴ ProN W3"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="12"/>
       <color indexed="8"/>
-      <name val="ヒラギノ角ゴ ProN W3"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
     </font>
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="ヒラギノ角ゴ ProN W6"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="ヒラギノ角ゴ ProN W3"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -126,29 +188,38 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -168,8 +239,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1401,336 +1471,373 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:I23"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozenSplit"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.03" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="9.05469" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.05469" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.05469" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.05469" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.05469" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.05469" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.05469" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.05469" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.05469" style="1" customWidth="1"/>
-    <col min="10" max="256" width="9.05469" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.125" style="1" customWidth="1"/>
+    <col min="10" max="256" width="9" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="23" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1"/>
-      <c r="C1"/>
-      <c r="D1"/>
-      <c r="E1"/>
-      <c r="F1"/>
-      <c r="G1"/>
-      <c r="H1"/>
-      <c r="I1"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="4"/>
     </row>
     <row r="2" ht="23.55" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="A2" t="s" s="5">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" t="s" s="6">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="C2" t="s" s="7">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="D2" t="s" s="6">
         <v>4</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="E2" t="s" s="6">
+        <v>5</v>
+      </c>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
     </row>
     <row r="3" ht="33.5" customHeight="1">
-      <c r="A3" s="4">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="9">
         <v>-200</v>
       </c>
-      <c r="C3" t="s" s="5">
+      <c r="C3" t="s" s="7">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s" s="9">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s" s="9">
+        <v>8</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" ht="33.3" customHeight="1">
+      <c r="A4" s="5">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s" s="7">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s" s="9">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s" s="9">
+        <v>9</v>
+      </c>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+    </row>
+    <row r="5" ht="33.3" customHeight="1">
+      <c r="A5" s="5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="9">
+        <v>200</v>
+      </c>
+      <c r="C5" t="s" s="7">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s" s="9">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+    </row>
+    <row r="6" ht="33.3" customHeight="1">
+      <c r="A6" s="5">
+        <v>4</v>
+      </c>
+      <c r="B6" s="9">
+        <v>1000</v>
+      </c>
+      <c r="C6" t="s" s="7">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s" s="9">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+    </row>
+    <row r="7" ht="33.3" customHeight="1">
+      <c r="A7" s="5">
         <v>5</v>
       </c>
-      <c r="D3" t="s" s="5">
+      <c r="B7" s="9">
+        <v>-200</v>
+      </c>
+      <c r="C7" t="s" s="7">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s" s="9">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s" s="9">
+        <v>12</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+    </row>
+    <row r="8" ht="33.3" customHeight="1">
+      <c r="A8" s="5">
         <v>6</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-    </row>
-    <row r="4" ht="33.3" customHeight="1">
-      <c r="A4" s="4">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5">
+      <c r="B8" s="9">
         <v>0</v>
       </c>
-      <c r="C4" t="s" s="5">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s" s="5">
+      <c r="C8" t="s" s="7">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s" s="9">
         <v>7</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-    </row>
-    <row r="5" ht="33.3" customHeight="1">
-      <c r="A5" s="4">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5">
+      <c r="E8" t="s" s="9">
+        <v>13</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+    </row>
+    <row r="9" ht="33.3" customHeight="1">
+      <c r="A9" s="5">
+        <v>7</v>
+      </c>
+      <c r="B9" s="9">
         <v>200</v>
       </c>
-      <c r="C5" t="s" s="5">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s" s="5">
+      <c r="C9" t="s" s="7">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s" s="9">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+    </row>
+    <row r="10" ht="33.3" customHeight="1">
+      <c r="A10" s="5">
         <v>8</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-    </row>
-    <row r="6" ht="33.3" customHeight="1">
-      <c r="A6" s="4">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5">
+      <c r="B10" s="9">
         <v>1000</v>
       </c>
-      <c r="C6" t="s" s="5">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s" s="5">
+      <c r="C10" t="s" s="7">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s" s="9">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+    </row>
+    <row r="11" ht="33.3" customHeight="1">
+      <c r="A11" s="5">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s" s="9">
+        <v>14</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" t="s" s="9">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s" s="9">
+        <v>12</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+    </row>
+    <row r="12" ht="33.3" customHeight="1">
+      <c r="A12" s="5">
+        <v>10</v>
+      </c>
+      <c r="B12" s="9">
+        <v>200</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="9">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s" s="9">
         <v>8</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-    </row>
-    <row r="7" ht="33.3" customHeight="1">
-      <c r="A7" s="4">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s" s="5">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s" s="5">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s" s="5">
-        <v>10</v>
-      </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-    </row>
-    <row r="8" ht="33.3" customHeight="1">
-      <c r="A8" s="4">
-        <v>6</v>
-      </c>
-      <c r="B8" s="5">
-        <v>200</v>
-      </c>
-      <c r="C8" s="5">
-        <v>10</v>
-      </c>
-      <c r="D8" t="s" s="5">
-        <v>6</v>
-      </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-    </row>
-    <row r="9" ht="23.35" customHeight="1">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-    </row>
-    <row r="10" ht="23.35" customHeight="1">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-    </row>
-    <row r="11" ht="23.35" customHeight="1">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-    </row>
-    <row r="12" ht="23.35" customHeight="1">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
     </row>
     <row r="13" ht="23.35" customHeight="1">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
     </row>
     <row r="14" ht="23.35" customHeight="1">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
     </row>
     <row r="15" ht="23.35" customHeight="1">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
     </row>
     <row r="16" ht="23.35" customHeight="1">
-      <c r="A16" s="4"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
     </row>
     <row r="17" ht="23.35" customHeight="1">
-      <c r="A17" s="4"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
     </row>
     <row r="18" ht="23.35" customHeight="1">
-      <c r="A18" s="4"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
     </row>
     <row r="19" ht="23.35" customHeight="1">
-      <c r="A19" s="4"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
     </row>
     <row r="20" ht="23.35" customHeight="1">
-      <c r="A20" s="4"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
+      <c r="A20" s="8"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
     </row>
     <row r="21" ht="23.35" customHeight="1">
-      <c r="A21" s="4"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
+      <c r="A21" s="8"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
     </row>
     <row r="22" ht="23.35" customHeight="1">
-      <c r="A22" s="4"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-    </row>
-    <row r="23" ht="23.35" customHeight="1">
-      <c r="A23" s="4"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
+      <c r="A22" s="8"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>